<commit_message>
Move manifest files to server code updated
</commit_message>
<xml_diff>
--- a/Move_FilesTo_Server/Data/Config.xlsx
+++ b/Move_FilesTo_Server/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NTMGRM.RPA1\Documents\UPProjects\Broadcast\Move_FilesTo_Server\Move_FilesTo_Server\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NTMGRM.RPA1\Documents\UPProjects\Move_FilesTo_Server\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9A5BB5-318F-4F63-98AE-4BD2DC93FCBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF02B5F8-6135-4B95-994B-215688D35B31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -28,55 +28,28 @@
     <t>Value</t>
   </si>
   <si>
-    <t>InputFALogFilePath</t>
+    <t>C:\Users\NTMGRM.RPA1\Documents\UPProjects\Broadcast\Brodcast to S9 data\</t>
   </si>
   <si>
-    <t>Parent Folder where all FA specific log files are stored</t>
+    <t>BroadcastFilesPath</t>
   </si>
   <si>
-    <t>OutputFALogFilePath</t>
+    <t>OOHFilePath</t>
   </si>
   <si>
-    <t>Output Parent Folder Where all FA specific log files will get stored</t>
+    <t>VendorFilePath</t>
   </si>
   <si>
-    <t>FALookup</t>
+    <t>PrintFilePath</t>
   </si>
   <si>
-    <t>Path of FA Lookup file</t>
+    <t>C:\Users\NTMGRM.RPA1\Documents\Print S9\zip\</t>
   </si>
   <si>
-    <t>ExceptionLogFilePath</t>
+    <t>C:\Users\NTMGRM.RPA1\Documents\UPProjects\OOH_S9\Data\manifest\zip\</t>
   </si>
   <si>
-    <t>Path of file where where all exception logs will get stored</t>
-  </si>
-  <si>
-    <t>SharePointURL</t>
-  </si>
-  <si>
-    <t>SharePointUser</t>
-  </si>
-  <si>
-    <t>SharePointPass</t>
-  </si>
-  <si>
-    <t>https://insidemedia.sharepoint.com/sites/GMUSA-InvoiceProcessing/</t>
-  </si>
-  <si>
-    <t>nycgrm.invoicebot@groupm.com</t>
-  </si>
-  <si>
-    <t>j3FWf75M</t>
-  </si>
-  <si>
-    <t>C:\1files\UPProjects\SquareNine\Files\Exception log file\</t>
-  </si>
-  <si>
-    <t>C:\1files\UPProjects\SquareNine\Files\Exclusion file.xlsx</t>
-  </si>
-  <si>
-    <t>C:\Users\NTMGRM.RPA1\Documents\UPProjects\Broadcast\Brodcast to S9 data\</t>
+    <t>C:\Users\NTMGRM.RPA1\Documents\UPProjects\Vendor S9\Vendor S9 Data\Vendor Manifest Data\zip\</t>
   </si>
 </sst>
 </file>
@@ -428,7 +401,7 @@
   <dimension ref="A1:Y994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -472,13 +445,10 @@
     </row>
     <row r="2" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -486,57 +456,35 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
     </row>
     <row r="8" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
+      <c r="A8" s="3"/>
     </row>
     <row r="9" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
@@ -1527,9 +1475,292 @@
     <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007D123EB44872014A9CBA28754C030F45" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b63aef4ab9a0554846bbd80426a442de">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a0a8f4a1-fec1-45cc-8c4b-70028d19f88b" xmlns:ns3="d1eda545-557d-4822-aebd-96c436cdfdd2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="025929af57d157df69a05cd96369afaf" ns2:_="" ns3:_="">
+    <xsd:import namespace="a0a8f4a1-fec1-45cc-8c4b-70028d19f88b"/>
+    <xsd:import namespace="d1eda545-557d-4822-aebd-96c436cdfdd2"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:Pic" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="a0a8f4a1-fec1-45cc-8c4b-70028d19f88b" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="11" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="12" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="14" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="17" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="18" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Pic" ma:index="19" nillable="true" ma:displayName="Pic" ma:format="Image" ma:internalName="Pic">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:URL">
+            <xsd:sequence>
+              <xsd:element name="Url" type="dms:ValidUrl" minOccurs="0" nillable="true"/>
+              <xsd:element name="Description" type="xsd:string" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="20" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="22" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="cb8c6112-a551-416c-b446-07c3fc3d0d42" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="d1eda545-557d-4822-aebd-96c436cdfdd2" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="15" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="16" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="23" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{818068d8-5dd5-4fbd-ae53-d04ba5fbca96}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="d1eda545-557d-4822-aebd-96c436cdfdd2">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Pic xmlns="a0a8f4a1-fec1-45cc-8c4b-70028d19f88b">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Pic>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a0a8f4a1-fec1-45cc-8c4b-70028d19f88b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d1eda545-557d-4822-aebd-96c436cdfdd2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17E162B7-10F4-440D-A82E-F114955F152D}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B024E980-492F-48F1-A213-AA516CC33B0F}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13A2891B-638C-4A77-995F-ED8080F03E15}"/>
 </file>
</xml_diff>